<commit_message>
Changed Roxie interpolation method and plot
</commit_message>
<xml_diff>
--- a/WMM_All_configurations/MCBXFB_02_Inner_Collar_600_20210510/Roxie_vs_MM_NormalMCBXFB_02_Inner_Collar_600_20210510.xlsx
+++ b/WMM_All_configurations/MCBXFB_02_Inner_Collar_600_20210510/Roxie_vs_MM_NormalMCBXFB_02_Inner_Collar_600_20210510.xlsx
@@ -617,6 +617,51 @@
       <c r="Q2">
         <v>0.2905807857671765</v>
       </c>
+      <c r="R2">
+        <v>-68.14581589863525</v>
+      </c>
+      <c r="S2">
+        <v>-3.020898060584047E-12</v>
+      </c>
+      <c r="T2">
+        <v>-0.3926034062378131</v>
+      </c>
+      <c r="U2">
+        <v>-5.170781728563633E-13</v>
+      </c>
+      <c r="V2">
+        <v>-0.0001764436175133731</v>
+      </c>
+      <c r="W2">
+        <v>2.961904231906723E-13</v>
+      </c>
+      <c r="X2">
+        <v>-7.408153680025089E-08</v>
+      </c>
+      <c r="Y2">
+        <v>2.720427668334274E-13</v>
+      </c>
+      <c r="Z2">
+        <v>-3.257876712706223E-11</v>
+      </c>
+      <c r="AA2">
+        <v>-1.047500611000503E-12</v>
+      </c>
+      <c r="AB2">
+        <v>8.878655506429485E-14</v>
+      </c>
+      <c r="AC2">
+        <v>8.354821097534107E-13</v>
+      </c>
+      <c r="AD2">
+        <v>-6.702843280855789E-13</v>
+      </c>
+      <c r="AE2">
+        <v>1.265817733494844E-12</v>
+      </c>
+      <c r="AF2">
+        <v>1.445312900633305E-13</v>
+      </c>
     </row>
     <row r="3" spans="1:32">
       <c r="A3" s="1">
@@ -671,49 +716,49 @@
         <v>0.2193344370488465</v>
       </c>
       <c r="R3">
-        <v>-155.2967770661369</v>
+        <v>3820.53361600509</v>
       </c>
       <c r="S3">
-        <v>-2.116667174537756E-11</v>
+        <v>-2.342903581552818E-12</v>
       </c>
       <c r="T3">
-        <v>6110.589996801313</v>
+        <v>-13.43056296579693</v>
       </c>
       <c r="U3">
-        <v>-1.930355102693977E-11</v>
+        <v>1.90026194601375E-12</v>
       </c>
       <c r="V3">
-        <v>-476.2957459097542</v>
+        <v>-56.58381757617198</v>
       </c>
       <c r="W3">
-        <v>-7.481416657415698E-12</v>
+        <v>3.434122951293175E-13</v>
       </c>
       <c r="X3">
-        <v>-81.94514303077051</v>
+        <v>-10.71440132254808</v>
       </c>
       <c r="Y3">
-        <v>-6.284689954729018E-13</v>
+        <v>-7.600284009294592E-13</v>
       </c>
       <c r="Z3">
-        <v>14.27561208430784</v>
+        <v>-1.451650138641211</v>
       </c>
       <c r="AA3">
-        <v>1.18928448060898E-11</v>
+        <v>7.681002117623181E-13</v>
       </c>
       <c r="AB3">
-        <v>1.104567898005908</v>
+        <v>-0.2105746429917907</v>
       </c>
       <c r="AC3">
-        <v>1.4674457049162E-11</v>
+        <v>7.950523979024575E-13</v>
       </c>
       <c r="AD3">
-        <v>-0.2901586217443245</v>
+        <v>-0.8379425932359311</v>
       </c>
       <c r="AE3">
-        <v>1.399895213979719E-11</v>
+        <v>-3.957146984635534E-14</v>
       </c>
       <c r="AF3">
-        <v>-0.07900385778879203</v>
+        <v>0.001623900910231786</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -769,49 +814,49 @@
         <v>0.2814318171014633</v>
       </c>
       <c r="R4">
-        <v>10000</v>
+        <v>10041.22891042461</v>
       </c>
       <c r="S4">
-        <v>-1.361064492927354E-13</v>
+        <v>-2.370740118676887E-13</v>
       </c>
       <c r="T4">
-        <v>-15.44569647566531</v>
+        <v>-15.38491883850872</v>
       </c>
       <c r="U4">
-        <v>2.050395588587869E-12</v>
+        <v>6.826304500105208E-13</v>
       </c>
       <c r="V4">
-        <v>0.2573915128266603</v>
+        <v>0.2337075053410519</v>
       </c>
       <c r="W4">
-        <v>2.286573963078398E-12</v>
+        <v>1.08336545256439E-13</v>
       </c>
       <c r="X4">
-        <v>2.22076240709662</v>
+        <v>2.221544324665985</v>
       </c>
       <c r="Y4">
-        <v>-2.102900982977703E-12</v>
+        <v>-6.650674399728485E-13</v>
       </c>
       <c r="Z4">
-        <v>3.245984176456485</v>
+        <v>3.229782662952247</v>
       </c>
       <c r="AA4">
-        <v>8.68628626228722E-13</v>
+        <v>-5.344701741907745E-13</v>
       </c>
       <c r="AB4">
-        <v>3.882282426276673</v>
+        <v>3.866729056542326</v>
       </c>
       <c r="AC4">
-        <v>-8.865979381443299E-13</v>
+        <v>1.348811853387962E-12</v>
       </c>
       <c r="AD4">
-        <v>-2.132102613282187</v>
+        <v>-2.123102370873716</v>
       </c>
       <c r="AE4">
-        <v>-4.138647806281467E-12</v>
+        <v>-9.855560844507763E-14</v>
       </c>
       <c r="AF4">
-        <v>0.4072932150563414</v>
+        <v>0.4053785506600061</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -867,49 +912,49 @@
         <v>0.3088349462494405</v>
       </c>
       <c r="R5">
-        <v>-59.09785251909443</v>
+        <v>3868.987338277233</v>
       </c>
       <c r="S5">
-        <v>-4.209964923143585E-12</v>
+        <v>-5.612616372746389E-13</v>
       </c>
       <c r="T5">
-        <v>8768.742561472809</v>
+        <v>-151.6735275080437</v>
       </c>
       <c r="U5">
-        <v>-4.055747131617732E-11</v>
+        <v>-1.22400683800898E-12</v>
       </c>
       <c r="V5">
-        <v>-1261.058899130722</v>
+        <v>-154.2990631783649</v>
       </c>
       <c r="W5">
-        <v>-4.675972545050516E-12</v>
+        <v>2.248537369836055E-13</v>
       </c>
       <c r="X5">
-        <v>-334.6590040124531</v>
+        <v>-45.0957393065293</v>
       </c>
       <c r="Y5">
-        <v>-2.771431283030814E-12</v>
+        <v>-9.179861597414763E-13</v>
       </c>
       <c r="Z5">
-        <v>-45.01231168000137</v>
+        <v>-13.75208624883947</v>
       </c>
       <c r="AA5">
-        <v>2.026036232329836E-11</v>
+        <v>-8.765724578276022E-14</v>
       </c>
       <c r="AB5">
-        <v>-24.24734269143748</v>
+        <v>-4.773636234195753</v>
       </c>
       <c r="AC5">
-        <v>2.946908251060466E-12</v>
+        <v>4.672726226891419E-13</v>
       </c>
       <c r="AD5">
-        <v>-10.25716705343176</v>
+        <v>-2.544962765292205</v>
       </c>
       <c r="AE5">
-        <v>1.75294203260425E-12</v>
+        <v>1.312381801705288E-12</v>
       </c>
       <c r="AF5">
-        <v>-3.708766717600412</v>
+        <v>-0.6290909285741511</v>
       </c>
     </row>
     <row r="6" spans="1:32">
@@ -963,6 +1008,51 @@
       </c>
       <c r="Q6">
         <v>0.2660522094574346</v>
+      </c>
+      <c r="R6">
+        <v>-65.15495286770917</v>
+      </c>
+      <c r="S6">
+        <v>6.995800346651404E-13</v>
+      </c>
+      <c r="T6">
+        <v>-1.86156742206555</v>
+      </c>
+      <c r="U6">
+        <v>-9.69570051032105E-13</v>
+      </c>
+      <c r="V6">
+        <v>-0.01064381918407512</v>
+      </c>
+      <c r="W6">
+        <v>1.349063820378472E-12</v>
+      </c>
+      <c r="X6">
+        <v>-0.0001093483097323885</v>
+      </c>
+      <c r="Y6">
+        <v>-8.286697816841414E-13</v>
+      </c>
+      <c r="Z6">
+        <v>-1.343989007620402E-06</v>
+      </c>
+      <c r="AA6">
+        <v>1.381745549908545E-12</v>
+      </c>
+      <c r="AB6">
+        <v>-1.826358344427081E-08</v>
+      </c>
+      <c r="AC6">
+        <v>4.18300106686472E-13</v>
+      </c>
+      <c r="AD6">
+        <v>-2.639729641896818E-10</v>
+      </c>
+      <c r="AE6">
+        <v>-6.315290763915076E-13</v>
+      </c>
+      <c r="AF6">
+        <v>-6.550721765202965E-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>